<commit_message>
Adding HW Ch1 through Ch02_Part_2; adding quizzes through week 4
</commit_message>
<xml_diff>
--- a/Grades.xlsx
+++ b/Grades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffberl/git/MCC/ENR261/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffberl/git/MCC/SP23_ENR261_Class/StephenBean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E346FE6C-947E-9349-A47E-704C22AB2071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B323CA30-8FD7-0D44-BD0C-D00829E08FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-32080" yWindow="6400" windowWidth="28040" windowHeight="17440" xr2:uid="{99F57567-4DED-EF46-8C44-7032F0DE2834}"/>
+    <workbookView xWindow="-30020" yWindow="5600" windowWidth="28040" windowHeight="17440" xr2:uid="{99F57567-4DED-EF46-8C44-7032F0DE2834}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="141">
   <si>
     <t>Tutorial_01_1</t>
   </si>
@@ -408,24 +408,6 @@
     <t>Ch02_1</t>
   </si>
   <si>
-    <t>No Errors</t>
-  </si>
-  <si>
-    <t>Grade Scale (per problem)</t>
-  </si>
-  <si>
-    <t>Minor Error</t>
-  </si>
-  <si>
-    <t>Major Error</t>
-  </si>
-  <si>
-    <t>Acceptable</t>
-  </si>
-  <si>
-    <t>7-8</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -493,9 +475,6 @@
   </si>
   <si>
     <t>Total</t>
-  </si>
-  <si>
-    <t>* assumes 100 for blank grades</t>
   </si>
   <si>
     <t>Simulink</t>
@@ -618,40 +597,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -674,6 +634,13 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -997,9 +964,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3A98D5-5F4A-C243-9D7E-CDA9B510E237}">
-  <dimension ref="A1:S17"/>
+  <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1010,7 +979,7 @@
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B1" s="20" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="20"/>
@@ -1026,154 +995,154 @@
       <c r="N1" s="20"/>
       <c r="O1" s="20"/>
       <c r="P1" s="2"/>
-      <c r="R1" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="S1" s="9"/>
+      <c r="R1" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="S1" s="18"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="14" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="14" t="s">
         <v>115</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="14" t="s">
         <v>114</v>
       </c>
-      <c r="E2" s="21" t="s">
+      <c r="E2" s="14" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="21" t="s">
+      <c r="F2" s="14" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="21" t="s">
+      <c r="G2" s="14" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="H2" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="I2" s="21" t="s">
+      <c r="I2" s="14" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="21" t="s">
+      <c r="J2" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="K2" s="21" t="s">
+      <c r="K2" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="L2" s="21" t="s">
+      <c r="L2" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="M2" s="21" t="s">
+      <c r="M2" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="N2" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="O2" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="P2" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="R2" s="7" t="s">
-        <v>126</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>127</v>
+      <c r="N2" s="14" t="s">
+        <v>140</v>
+      </c>
+      <c r="O2" s="14" t="s">
+        <v>139</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="14" t="str">
-        <f ca="1">IF(COUNT(INDIRECT("'"&amp;B$2&amp;"'!$B:$B"))=0,"",SUMIF(INDIRECT("'"&amp;B$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;B$2&amp;"'!$B:$B"))/(COUNTIFS(INDIRECT("'"&amp;B$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;B$2&amp;"'!$C:$C"),"")*10))</f>
+      <c r="B3" s="16">
+        <f ca="1">IF(COUNT(INDIRECT("'"&amp;B$2&amp;"'!$B:$B"))=0,"",SUMIF(INDIRECT("'"&amp;B$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;B$2&amp;"'!$B:$B"))/(COUNTIFS(INDIRECT("'"&amp;B$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;B$2&amp;"'!$C:$C"),"")))</f>
+        <v>1</v>
+      </c>
+      <c r="C3" s="16" t="str">
+        <f t="shared" ref="C3:O3" ca="1" si="0">IF(COUNT(INDIRECT("'"&amp;C$2&amp;"'!$B:$B"))=0,"",SUMIF(INDIRECT("'"&amp;C$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;C$2&amp;"'!$B:$B"))/(COUNTIFS(INDIRECT("'"&amp;C$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;C$2&amp;"'!$C:$C"),"")))</f>
         <v/>
       </c>
-      <c r="C3" s="14" t="str">
-        <f t="shared" ref="C3:O3" ca="1" si="0">IF(COUNT(INDIRECT("'"&amp;C$2&amp;"'!$B:$B"))=0,"",SUMIF(INDIRECT("'"&amp;C$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;C$2&amp;"'!$B:$B"))/(COUNTIFS(INDIRECT("'"&amp;C$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;C$2&amp;"'!$C:$C"),"")*10))</f>
-        <v/>
-      </c>
-      <c r="D3" s="14" t="str">
+      <c r="D3" s="16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="E3" s="14" t="str">
+      <c r="F3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="F3" s="14" t="str">
+      <c r="G3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="G3" s="14" t="str">
+      <c r="H3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="H3" s="14" t="str">
+      <c r="I3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="I3" s="14" t="str">
+      <c r="J3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="J3" s="14" t="str">
+      <c r="K3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="K3" s="14" t="str">
+      <c r="L3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="L3" s="14" t="str">
+      <c r="M3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="M3" s="14" t="str">
+      <c r="N3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="N3" s="14" t="str">
+      <c r="O3" s="16" t="str">
         <f t="shared" ca="1" si="0"/>
         <v/>
       </c>
-      <c r="O3" s="14" t="str">
-        <f t="shared" ca="1" si="0"/>
-        <v/>
-      </c>
-      <c r="P3" s="18" t="str">
+      <c r="P3" s="11">
         <f ca="1">IF(ISERROR(IF(PROJ_GRADE&gt;MIN(HW_GRADES),SUM(HW_GRADES)-MIN(HW_GRADES)+PROJ_GRADE/COUNT(HW_GRADES),AVERAGE(HW_GRADES))),"",IF(PROJ_GRADE&gt;MIN(HW_GRADES),SUM(HW_GRADES)-MIN(HW_GRADES)+PROJ_GRADE/COUNT(HW_GRADES),AVERAGE(HW_GRADES)))</f>
-        <v/>
-      </c>
-      <c r="R3" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="R3" s="4">
         <v>0</v>
       </c>
-      <c r="S3" s="7" t="s">
-        <v>128</v>
+      <c r="S3" s="5" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="R4" s="6">
+      <c r="R4" s="4">
         <v>57</v>
       </c>
-      <c r="S4" s="7" t="s">
-        <v>129</v>
+      <c r="S4" s="5" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="R5" s="6">
+      <c r="R5" s="4">
         <v>60</v>
       </c>
-      <c r="S5" s="7" t="s">
-        <v>130</v>
+      <c r="S5" s="5" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
-        <v>124</v>
+      <c r="B6" s="19" t="s">
+        <v>118</v>
       </c>
       <c r="C6" s="20"/>
       <c r="D6" s="20"/>
@@ -1186,163 +1155,167 @@
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="P6" s="2"/>
-      <c r="R6" s="6">
+      <c r="R6" s="4">
         <v>64</v>
       </c>
-      <c r="S6" s="7" t="s">
+      <c r="S6" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B7" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I7" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="L7" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="M7" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="R7" s="4">
+        <v>67</v>
+      </c>
+      <c r="S7" s="5" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9">
+        <v>0.95</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9">
+        <v>1</v>
+      </c>
+      <c r="F8" s="9">
+        <v>0.79169999999999996</v>
+      </c>
+      <c r="G8" s="9"/>
+      <c r="H8" s="9"/>
+      <c r="I8" s="9"/>
+      <c r="J8" s="9"/>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="11">
+        <f>IF(ISERROR(IF(PROJ_GRADE&gt;MIN(QUIZ_GRADES),(SUM(QUIZ_GRADES)-MIN(QUIZ_GRADES)+PROJ_GRADE)/COUNT(QUIZ_GRADES),AVERAGE(QUIZ_GRADES))),"",IF(PROJ_GRADE&gt;MIN(QUIZ_GRADES),(SUM(QUIZ_GRADES)-MIN(QUIZ_GRADES)+PROJ_GRADE)/COUNT(QUIZ_GRADES),AVERAGE(QUIZ_GRADES)))</f>
+        <v>0.94833999999999996</v>
+      </c>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="R8" s="4">
+        <v>70</v>
+      </c>
+      <c r="S8" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M9" s="10"/>
+      <c r="R9" s="4">
+        <v>74</v>
+      </c>
+      <c r="S9" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R10" s="4">
+        <v>77</v>
+      </c>
+      <c r="S10" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="R11" s="4">
+        <v>80</v>
+      </c>
+      <c r="S11" s="5" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="B12" s="15"/>
+      <c r="R12" s="4">
+        <v>85</v>
+      </c>
+      <c r="S12" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A7" s="10"/>
-      <c r="B7" s="21" t="s">
-        <v>104</v>
-      </c>
-      <c r="C7" s="21" t="s">
-        <v>115</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E7" s="21" t="s">
-        <v>105</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>106</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>107</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" s="21" t="s">
-        <v>109</v>
-      </c>
-      <c r="J7" s="21" t="s">
-        <v>110</v>
-      </c>
-      <c r="K7" s="21" t="s">
-        <v>113</v>
-      </c>
-      <c r="L7" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="M7" s="12" t="s">
-        <v>144</v>
-      </c>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="R7" s="6">
-        <v>67</v>
-      </c>
-      <c r="S7" s="7" t="s">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R13" s="4">
+        <v>90</v>
+      </c>
+      <c r="S13" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16"/>
-      <c r="I8" s="16"/>
-      <c r="J8" s="16"/>
-      <c r="K8" s="16"/>
-      <c r="L8" s="16"/>
-      <c r="M8" s="18" t="str">
-        <f>IF(ISERROR(IF(PROJ_GRADE&gt;MIN(QUIZ_GRADES),(SUM(QUIZ_GRADES)-MIN(QUIZ_GRADES)+PROJ_GRADE)/COUNT(QUIZ_GRADES),AVERAGE(QUIZ_GRADES))),"",IF(PROJ_GRADE&gt;MIN(QUIZ_GRADES),(SUM(QUIZ_GRADES)-MIN(QUIZ_GRADES)+PROJ_GRADE)/COUNT(QUIZ_GRADES),AVERAGE(QUIZ_GRADES)))</f>
-        <v/>
-      </c>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="R8" s="6">
-        <v>70</v>
-      </c>
-      <c r="S8" s="7" t="s">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="R14" s="4">
+        <v>93</v>
+      </c>
+      <c r="S14" s="5" t="s">
         <v>133</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="M9" s="17"/>
-      <c r="R9" s="6">
-        <v>74</v>
-      </c>
-      <c r="S9" s="7" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="R10" s="6">
-        <v>77</v>
-      </c>
-      <c r="S10" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="B11" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="R11" s="6">
-        <v>80</v>
-      </c>
-      <c r="S11" s="7" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B12" s="22"/>
-      <c r="R12" s="6">
-        <v>85</v>
-      </c>
-      <c r="S12" s="7" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="R13" s="6">
-        <v>90</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="R14" s="6">
-        <v>93</v>
-      </c>
-      <c r="S14" s="7" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.2">
       <c r="G15" s="20" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="H15" s="20"/>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="G16" s="19">
+      <c r="G16" s="12">
         <f ca="1">IF(TOTAL_PROJ_GRADE="",1,TOTAL_PROJ_GRADE)*0.4+IF(TOTAL_QUIZ_GRADE="",1,TOTAL_QUIZ_GRADE)*0.4+IF(TOTAL_HW_GRADE="",1,TOTAL_HW_GRADE)*0.2</f>
-        <v>1</v>
-      </c>
-      <c r="H16" s="11" t="str">
+        <v>0.87933600000000001</v>
+      </c>
+      <c r="H16" s="6" t="str">
         <f ca="1">INDEX(LETTER_GRADES,MATCH(OVERALL_GRADE*100,SCALAR_GRADES,1),0)</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
-      <c r="G17" t="s">
-        <v>145</v>
+        <v>B+</v>
       </c>
     </row>
   </sheetData>
@@ -1359,9 +1332,11 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{839D11EB-772C-1D48-92B5-81EA03F65E13}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1379,38 +1354,92 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>62</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>63</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>66</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>67</v>
       </c>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1420,9 +1449,11 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35E3892-960F-6046-898C-CF17FBB93C28}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1440,48 +1471,98 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>68</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>70</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>71</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>72</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>73</v>
       </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>74</v>
       </c>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>75</v>
       </c>
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1491,9 +1572,11 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52781228-C733-5F41-8F38-602D7F51F82A}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1511,43 +1594,95 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>76</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>77</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>78</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>79</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>80</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>81</v>
       </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>82</v>
       </c>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1557,9 +1692,11 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2497D3C3-6A1A-194F-809C-E8E63B41492E}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1577,46 +1714,98 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>83</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>84</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>85</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>86</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>87</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>88</v>
       </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>89</v>
       </c>
+      <c r="B8" s="17"/>
       <c r="C8" t="s">
         <v>90</v>
       </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1626,9 +1815,11 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C9E36D-48F1-8D42-98FB-6D6CB04E6B98}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1646,33 +1837,89 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>91</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>92</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>93</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>94</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>95</v>
       </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1681,9 +1928,11 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1FE5C4A-1757-AC44-A715-4D9E72D718D9}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1701,43 +1950,50 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>96</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>97</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>98</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>99</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>100</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>101</v>
       </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>102</v>
       </c>
+      <c r="B8" s="17"/>
       <c r="C8" t="s">
         <v>90</v>
       </c>
@@ -1746,17 +2002,58 @@
       <c r="A9" s="1" t="s">
         <v>103</v>
       </c>
+      <c r="B9" s="17"/>
       <c r="C9" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>140</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B10" s="17"/>
       <c r="C10" t="s">
         <v>90</v>
       </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1766,7 +2063,631 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{272F2D5C-3177-5B49-A205-195CA8F1D25F}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CB1B56-5F0D-C74E-AED3-ACBF7434713C}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE37708F-8731-5243-9374-1137F30798A7}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9232FB-4DAB-754B-AA2C-CF09C5F96E42}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5964A636-510B-DF40-8DF8-97FD394BEC03}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="4" max="4" width="51.1640625" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="17"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="17"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="17"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="17"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="17"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="17"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="17"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245CF9CF-42D7-D54A-8B09-914D665A9F90}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1780,93 +2701,6 @@
     <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G1" s="8"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="G2" s="3">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="G3" s="3">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="G5" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="F1:G1"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87CB1B56-5F0D-C74E-AED3-ACBF7434713C}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>5</v>
@@ -1875,326 +2709,101 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE37708F-8731-5243-9374-1137F30798A7}">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F9232FB-4DAB-754B-AA2C-CF09C5F96E42}">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5964A636-510B-DF40-8DF8-97FD394BEC03}">
-  <dimension ref="A1:D6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{245CF9CF-42D7-D54A-8B09-914D665A9F90}">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
-    <col min="4" max="4" width="51.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>90</v>
-      </c>
-      <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>36</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>37</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>38</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>39</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>40</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>41</v>
       </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>42</v>
       </c>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>43</v>
       </c>
+      <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>44</v>
       </c>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2204,9 +2813,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85ED12DE-DE96-BB4D-8C1C-CD7E8835D4AD}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2225,48 +2836,98 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>45</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>46</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>47</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>48</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>49</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>50</v>
       </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>51</v>
       </c>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>52</v>
       </c>
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2276,9 +2937,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4FEC51AF-2F0F-9B4D-A92A-F7DE266B2F52}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -2296,53 +2959,101 @@
         <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>53</v>
       </c>
+      <c r="B2" s="17"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>54</v>
       </c>
+      <c r="B3" s="17"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>55</v>
       </c>
+      <c r="B4" s="17"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>56</v>
       </c>
+      <c r="B5" s="17"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>57</v>
       </c>
+      <c r="B6" s="17"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>58</v>
       </c>
+      <c r="B7" s="17"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>59</v>
       </c>
+      <c r="B8" s="17"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>60</v>
       </c>
+      <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>61</v>
       </c>
+      <c r="B10" s="17"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="17"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="17"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="17"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="17"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="17"/>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="17"/>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="17"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="17"/>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="17"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="17"/>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="17"/>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="17"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
Fixing Chapter 2 Part 2 Grades
</commit_message>
<xml_diff>
--- a/Grades.xlsx
+++ b/Grades.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffberl/git/MCC/SP23_ENR261_Class/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/geoffberl/git/MCC/SP23_ENR261_Class/StephenBean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796C4391-ABE9-0842-BE46-64743E7F6B4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11453584-0884-1647-8721-12F8D644DCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41440" yWindow="7600" windowWidth="28040" windowHeight="17440"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19960" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="2" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>Tutorial_02_05</t>
-  </si>
-  <si>
     <t>Program_02_1</t>
   </si>
   <si>
@@ -99,18 +96,6 @@
     <t>Program_02_6</t>
   </si>
   <si>
-    <t>Tutorial_02_06</t>
-  </si>
-  <si>
-    <t>Tutorial_02_07</t>
-  </si>
-  <si>
-    <t>Tutorial_02_08</t>
-  </si>
-  <si>
-    <t>Tutorial_02_09</t>
-  </si>
-  <si>
     <t>Program_02_7</t>
   </si>
   <si>
@@ -387,15 +372,6 @@
     <t>Ch02_Part2</t>
   </si>
   <si>
-    <t>Incorrect output</t>
-  </si>
-  <si>
-    <t>Outputs are incorrect, most should be vectors but your results are scalars.</t>
-  </si>
-  <si>
-    <t>See expected output</t>
-  </si>
-  <si>
     <t>Tutorial_07_9</t>
   </si>
   <si>
@@ -403,6 +379,30 @@
   </si>
   <si>
     <t>Program_10_2</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>Not found</t>
+  </si>
+  <si>
+    <t>Tutorial_02_5</t>
+  </si>
+  <si>
+    <t>Tutorial_02_6</t>
+  </si>
+  <si>
+    <t>Tutorial_02_7</t>
+  </si>
+  <si>
+    <t>Tutorial_02_8</t>
+  </si>
+  <si>
+    <t>Tutorial_02_9</t>
   </si>
   <si>
     <t>Not found</t>
@@ -898,24 +898,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC3A98D5-5F4A-C243-9D7E-CDA9B510E237}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="true" zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="9.140625" customWidth="true"/>
+    <col min="2" max="2" width="9.1640625" customWidth="true"/>
     <col min="3" max="3" width="12" customWidth="true"/>
-    <col min="5" max="5" width="9.140625" customWidth="true"/>
+    <col min="5" max="8" width="9.1640625" customWidth="true"/>
     <col min="18" max="18" width="15.83203125" bestFit="true" customWidth="true"/>
     <col min="19" max="19" width="12.6640625" customWidth="true"/>
     <col min="20" max="20" width="10.6640625" customWidth="true"/>
     <col min="4" max="4" width="12" customWidth="true"/>
-    <col min="6" max="6" width="9.140625" customWidth="true"/>
-    <col min="7" max="8" width="9.1640625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
       <c r="B1" s="19" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C1" s="19"/>
       <c r="D1" s="19"/>
@@ -932,86 +930,86 @@
       <c r="O1" s="19"/>
       <c r="P1" s="1"/>
       <c r="R1" s="17" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="S1" s="17"/>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E2" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="G2" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H2" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="K2" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="L2" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="M2" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="N2" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="O2" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="F2" s="13" t="s">
-        <v>79</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="H2" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="I2" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="J2" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="K2" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="L2" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="M2" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="N2" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="O2" s="13" t="s">
-        <v>102</v>
-      </c>
-      <c r="P2" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="S2" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="15" t="str">
+      <c r="B3" s="15">
         <f ca="true">IF(COUNT(INDIRECT("'"&amp;B$2&amp;"'!$B:$B"))=0,"",SUMIF(INDIRECT("'"&amp;B$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;B$2&amp;"'!$B:$B"))/(COUNTIFS(INDIRECT("'"&amp;B$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;B$2&amp;"'!$C:$C"),"")))</f>
-        <v/>
-      </c>
-      <c r="C3" s="15" t="str">
+        <v>1</v>
+      </c>
+      <c r="C3" s="15">
         <f t="shared" ref="C3:O3" ca="true" si="0">IF(COUNT(INDIRECT("'"&amp;C$2&amp;"'!$B:$B"))=0,"",SUMIF(INDIRECT("'"&amp;C$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;C$2&amp;"'!$B:$B"))/(COUNTIFS(INDIRECT("'"&amp;C$2&amp;"'!$A:$A"),"&lt;&gt;"&amp;"",INDIRECT("'"&amp;C$2&amp;"'!$C:$C"),"")))</f>
-        <v/>
-      </c>
-      <c r="D3" s="15" t="str">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D3" s="15">
         <f t="shared" ca="true" si="0"/>
-        <v/>
-      </c>
-      <c r="E3" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="E3" s="15">
         <f t="shared" ca="true" si="0"/>
-        <v/>
-      </c>
-      <c r="F3" s="15" t="str">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
         <f t="shared" ca="true" si="0"/>
-        <v/>
+        <v>0</v>
       </c>
       <c r="G3" s="15" t="str">
         <f t="shared" ca="true" si="0"/>
@@ -1049,15 +1047,15 @@
         <f t="shared" ca="true" si="0"/>
         <v/>
       </c>
-      <c r="P3" s="10" t="str">
+      <c r="P3" s="10">
         <f ca="true">IF(ISERROR(IF(PROJ_GRADE&gt;MIN(HW_GRADES),SUM(HW_GRADES)-MIN(HW_GRADES)+PROJ_GRADE/COUNT(HW_GRADES),AVERAGE(HW_GRADES))),"",IF(PROJ_GRADE&gt;MIN(HW_GRADES),SUM(HW_GRADES)-MIN(HW_GRADES)+PROJ_GRADE/COUNT(HW_GRADES),AVERAGE(HW_GRADES)))</f>
-        <v/>
+        <v>0.42000000000000004</v>
       </c>
       <c r="R3" s="3">
         <v>0</v>
       </c>
       <c r="S3" s="4" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
@@ -1065,7 +1063,7 @@
         <v>57</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
@@ -1073,12 +1071,12 @@
         <v>60</v>
       </c>
       <c r="S5" s="4" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="C6" s="19"/>
       <c r="D6" s="19"/>
@@ -1095,45 +1093,45 @@
         <v>64</v>
       </c>
       <c r="S6" s="4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G7" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="K7" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="L7" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="I7" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>97</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>98</v>
-      </c>
-      <c r="L7" s="13" t="s">
-        <v>99</v>
-      </c>
       <c r="M7" s="6" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="N7" s="6"/>
       <c r="O7" s="6"/>
@@ -1141,7 +1139,7 @@
         <v>67</v>
       </c>
       <c r="S7" s="4" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
@@ -1169,9 +1167,9 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
       <c r="L8" s="8"/>
-      <c r="M8" s="10" t="str">
+      <c r="M8" s="10">
         <f>IF(ISERROR(IF(PROJ_GRADE&gt;MIN(QUIZ_GRADES),(SUM(QUIZ_GRADES)-MIN(QUIZ_GRADES)+PROJ_GRADE)/COUNT(QUIZ_GRADES),AVERAGE(QUIZ_GRADES))),"",IF(PROJ_GRADE&gt;MIN(QUIZ_GRADES),(SUM(QUIZ_GRADES)-MIN(QUIZ_GRADES)+PROJ_GRADE)/COUNT(QUIZ_GRADES),AVERAGE(QUIZ_GRADES)))</f>
-        <v/>
+        <v>0.99</v>
       </c>
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
@@ -1179,7 +1177,7 @@
         <v>70</v>
       </c>
       <c r="S8" s="4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.2">
@@ -1188,7 +1186,7 @@
         <v>74</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.2">
@@ -1196,30 +1194,30 @@
         <v>77</v>
       </c>
       <c r="S10" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="R11" s="3">
         <v>80</v>
       </c>
       <c r="S11" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B12" s="14"/>
       <c r="R12" s="3">
         <v>85</v>
       </c>
       <c r="S12" s="4" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.2">
@@ -1227,7 +1225,7 @@
         <v>90</v>
       </c>
       <c r="S13" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.2">
@@ -1235,23 +1233,23 @@
         <v>93</v>
       </c>
       <c r="S14" s="4" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" x14ac:dyDescent="0.2">
       <c r="G15" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="H15" s="19"/>
     </row>
     <row r="16" x14ac:dyDescent="0.2">
       <c r="G16" s="11">
         <f ca="true">IF(TOTAL_PROJ_GRADE="",1,TOTAL_PROJ_GRADE)*0.4+IF(TOTAL_QUIZ_GRADE="",1,TOTAL_QUIZ_GRADE)*0.4+IF(TOTAL_HW_GRADE="",1,TOTAL_HW_GRADE)*0.2</f>
-        <v>1</v>
+        <v>0.88000000000000012</v>
       </c>
       <c r="H16" s="5" t="str">
         <f ca="true">INDEX(LETTER_GRADES,MATCH(OVERALL_GRADE*100,SCALAR_GRADES,1),0)</f>
-        <v>A</v>
+        <v>B+</v>
       </c>
     </row>
   </sheetData>
@@ -1286,35 +1284,35 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1343,45 +1341,45 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1409,20 +1407,20 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1447,10 +1445,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1474,10 +1472,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1501,10 +1499,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -1521,9 +1519,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.1640625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="9.140625" style="16" customWidth="true"/>
+    <col min="2" max="2" width="9.1640625" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="6.7109375" customWidth="true"/>
+    <col min="4" max="4" width="6.6640625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.2">
@@ -1531,10 +1529,10 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
@@ -1544,7 +1542,6 @@
       <c r="B2" s="16">
         <v>1</v>
       </c>
-      <c r="D2" s="0"/>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
@@ -1553,7 +1550,6 @@
       <c r="B3" s="16">
         <v>1</v>
       </c>
-      <c r="D3" s="0"/>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -1562,7 +1558,6 @@
       <c r="B4" s="16">
         <v>1</v>
       </c>
-      <c r="D4" s="0"/>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
@@ -1571,7 +1566,6 @@
       <c r="B5" s="16">
         <v>1</v>
       </c>
-      <c r="D5" s="0"/>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
@@ -1580,7 +1574,6 @@
       <c r="B6" s="16">
         <v>1</v>
       </c>
-      <c r="D6" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1597,9 +1590,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.5" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="6.85546875" style="16" customWidth="true"/>
+    <col min="2" max="2" width="10.33203125" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="6.7109375" customWidth="true"/>
+    <col min="4" max="4" width="6.6640625" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1608,101 +1601,91 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B2" s="16">
-        <v>0</v>
-      </c>
-      <c r="D2" s="0"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B3" s="16">
         <v>0</v>
       </c>
-      <c r="D3" s="0"/>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
       </c>
-      <c r="D4" s="0"/>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B5" s="16">
         <v>0</v>
       </c>
-      <c r="D5" s="0"/>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="16">
         <v>0</v>
       </c>
-      <c r="D6" s="0"/>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="16">
         <v>0</v>
       </c>
-      <c r="D7" s="0"/>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
       </c>
-      <c r="D8" s="0"/>
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="16">
         <v>0</v>
       </c>
-      <c r="D9" s="0"/>
     </row>
     <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B10" s="16">
         <v>0</v>
       </c>
-      <c r="D10" s="0"/>
     </row>
     <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B11" s="16">
         <v>0</v>
       </c>
-      <c r="D11" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1714,7 +1697,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE37708F-8731-5243-9374-1137F30798A7}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="true" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1730,40 +1715,60 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B2" s="16">
+        <v>0</v>
+      </c>
+      <c r="D2" s="0"/>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>13</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0</v>
+      </c>
+      <c r="D3" s="0"/>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>14</v>
-      </c>
+        <v>112</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0</v>
+      </c>
+      <c r="D4" s="0"/>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>15</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0"/>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>16</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="B6" s="16">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0"/>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B7" s="16">
         <v>0</v>
@@ -1774,7 +1779,7 @@
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -1785,7 +1790,7 @@
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B9" s="16">
         <v>0</v>
@@ -1808,9 +1813,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="6.85546875" style="16" customWidth="true"/>
+    <col min="2" max="2" width="6.83203125" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="6.7109375" customWidth="true"/>
+    <col min="4" max="4" width="6.6640625" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1819,38 +1824,35 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B2" s="16">
         <v>0</v>
       </c>
-      <c r="D2" s="0"/>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B3" s="16">
         <v>0</v>
       </c>
-      <c r="D3" s="0"/>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
       </c>
-      <c r="D4" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1867,9 +1869,9 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.1640625" bestFit="true" customWidth="true"/>
-    <col min="2" max="2" width="6.85546875" style="16" customWidth="true"/>
+    <col min="2" max="2" width="6.83203125" style="16" customWidth="true"/>
     <col min="3" max="3" width="11" customWidth="true"/>
-    <col min="4" max="4" width="6.7109375" customWidth="true"/>
+    <col min="4" max="4" width="6.6640625" customWidth="true"/>
     <col min="7" max="7" width="12" customWidth="true"/>
   </cols>
   <sheetData>
@@ -1878,56 +1880,51 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B2" s="16">
         <v>0</v>
       </c>
-      <c r="D2" s="0"/>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B3" s="16">
         <v>0</v>
       </c>
-      <c r="D3" s="0"/>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B4" s="16">
         <v>0</v>
       </c>
-      <c r="D4" s="0"/>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B5" s="16">
         <v>0</v>
       </c>
-      <c r="D5" s="0"/>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B6" s="16">
         <v>0</v>
       </c>
-      <c r="D6" s="0"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -1955,65 +1952,65 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2042,35 +2039,35 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -2099,75 +2096,75 @@
         <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>